<commit_message>
Them tai lieu scalping
</commit_message>
<xml_diff>
--- a/Breakout.xlsx
+++ b/Breakout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="157">
   <si>
     <t>Người thực hiện:</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Nội dung</t>
   </si>
   <si>
-    <t>Bắt những pha khi thị trường phá đỉnh hoặc phá đáy</t>
-  </si>
-  <si>
     <t>Khung thời gian H4, H1, M15</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>giờ khi giá đã chạm vào đường MA55 thì ta sẽ thấy được các ngưỡng hỗ trợ và kháng cự xuất hiện bao khu vực này</t>
-  </si>
-  <si>
     <t>ta kẻ các ngưỡng đó ra</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>chú ý là phải tính từ cái râu nến nha, thiếu râu nến là toang luôn và ngay đấy</t>
   </si>
   <si>
-    <t>Đó là những đáy, đỉnh của những xu hướng lớn đã hình thành trước đó</t>
-  </si>
-  <si>
     <t>hay một chỉ báo nào cho thấy thị trường đang phân phối hay tích lũy cũng được</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>khi có cái râu nến mới mà cao hơn hay thấp hơn các ngưỡng thì phải cập nhật cái râu nến mới đó vào làm ngưỡng mới nha</t>
   </si>
   <si>
-    <t>khi giá cắt qua đường MA55 rồi hồi lại thì sẽ hình thành một cái ngưỡng, ta sẽ so với cái ngưỡng gần nhất rồi cập nhật theo cái nào cao hơn hay thấp hơn nha</t>
-  </si>
-  <si>
     <t xml:space="preserve">ta chờ đến khi giá hội tụ với đường MA55 thì ta sẽ biết được cái đáy hay đỉnh và ta sẽ đặt takeprofit ở gần cái đáy hay đỉnh đó, do nguyên lý giá sẽ retest lại cái đáy hay đỉnh mới </t>
   </si>
   <si>
@@ -360,17 +348,155 @@
     <t>Trade theo xu hướng bắt sóng hồi và vào lệnh(nâng cao)</t>
   </si>
   <si>
-    <t>Khi giá phá đỉnh thì mua, phá đáy thì bán(Cơ bản)</t>
-  </si>
-  <si>
     <t>Do giao dịch theo phương pháp breakout nên nếu xác định các ngưỡng mà sai thì sẽ dẫn tới hiện tượng xác định breakout sai(cực kỳ nguy hiểm)</t>
+  </si>
+  <si>
+    <t>khi giá cắt qua đường MA55 rồi hồi lại thì sẽ hình thành một cái ngưỡng, ta sẽ so với cái ngưỡng gần nhất rồi cập nhật theo cái nào cao hơn hay thấp hơn nha (Như hình dưới)</t>
+  </si>
+  <si>
+    <t>Để đảm bảo vị thế vững chắc khi vào lệnh thì ta phải đảm bao thêm một số điều kiện sau</t>
+  </si>
+  <si>
+    <t>Bật khung H1 lên</t>
+  </si>
+  <si>
+    <t>Sau đó giá sẽ test lại keylevel một lần nữa</t>
+  </si>
+  <si>
+    <t>Khi này nó sẽ hình thành vùng RT</t>
+  </si>
+  <si>
+    <t>Thì ta sẽ vào lệnh khi giá phá qua RT</t>
+  </si>
+  <si>
+    <t>Dựa vào điều này cũng tăng cường vị thế cho lệnh khi breakout xảy ra</t>
+  </si>
+  <si>
+    <t>Nếu không đảm bảo điều kiện này thì có thể ta sẽ gặp phải breakout nếu xuất hiện một cây nến H1 nằm ngang qua keylevel</t>
+  </si>
+  <si>
+    <t>Hoặc xuất hiện những cây nến pinbar hay doji hay sao mai ở vùng này</t>
+  </si>
+  <si>
+    <t>Nghĩa là những cây nến H1 khi vào vùng này thì thường bị chững lại, có thế có râu nến cắt qua keylevel</t>
+  </si>
+  <si>
+    <t>Nếu nâng cao hơn thì ta chờ giá retest lại keylevel vừa phá để tăng cường RR</t>
+  </si>
+  <si>
+    <t>Những cây nến nằm ngang dó thường là những cây nến marubozu to dài và khỏe :))</t>
+  </si>
+  <si>
+    <t>Thì khi này ta chỉ việc buy hoặc sell theo nến thôi, nghĩ nhiều làm gì</t>
+  </si>
+  <si>
+    <t>khi giá vừa vào vùng keylevel mà có dấu hiệu chững lại thì ta không được vào lệnh ngay nha</t>
+  </si>
+  <si>
+    <t>ta phải chờ vài ba cây nến và xuất hiện nến đảo chiều đủ mạnh thì mới vào lệnh</t>
+  </si>
+  <si>
+    <t>nếu không khi gặp ngay cây breakout là tạch luôn</t>
+  </si>
+  <si>
+    <t>còn nếu gặp cây breakout thì cứ mạnh dạn bơi theo nó luôn do khi breakout giá sẽ đi nhanh và mạnh, không chờ một ai đâu</t>
+  </si>
+  <si>
+    <t>Phải xem phần bổ sung(Xuất hiện nến đảo chiều ở khung H1) ở phần dưới này để đảm bảo vị thế khi vào lệnh</t>
+  </si>
+  <si>
+    <t>Xem phần bổ xung để tăng vị thế khi take profit</t>
+  </si>
+  <si>
+    <t>Nếu ta có một vị thế tốt khi vào lệnh ở vùng keylevel dưới, ta sẽ xem giá phản ứng ở vùng keylevel trên như thế nào để tiến hành takeprofit sau cho tăng tỷ lệ RR hoặc giảm rủi ro</t>
+  </si>
+  <si>
+    <t>Nghĩa là vào lệnh chờ giá đi đến keylevel phía trên</t>
+  </si>
+  <si>
+    <t>Nếu giá không phá được keylevel đó mà có dấu hiệu đảo chiều thì ta sẽ takeprofit ở keylevel đó</t>
+  </si>
+  <si>
+    <t>Nếu giá cắt qua keylevel đó thì ta chỉ việc gồng lời tiếp thôi</t>
+  </si>
+  <si>
+    <t>Chú ý là dựa trên khung H1 nha</t>
+  </si>
+  <si>
+    <t>Chú ý là khi giá vào vùng key level mà bị bật lại thì nó sẽ vào vùng keylevel kia( khả năng cao là thế)</t>
+  </si>
+  <si>
+    <t>Vì vậy cần phải xác định đúng keylevel, nếu xác định sai thì sẽ tính toán sai</t>
+  </si>
+  <si>
+    <t>Keylevel ở khung thời gian càng cao thì càng chuẩn xác, ít nhất là từ H1, H4 đổ lên</t>
+  </si>
+  <si>
+    <t>Mấy cái keylevel ở khung thời gian thấp toàn là rác, nhiều nhiễu</t>
+  </si>
+  <si>
+    <t>Đối với nến M15 thì phải chờ retest rồi phá</t>
+  </si>
+  <si>
+    <t>Còn nâng cao hơn là khi nến M15 phá thì chờ nến H1 hình thành và có thân nằm ngang trên ngưỡng thì đảm bảo cho breakout thành công thì chỉ cần vào lệnh theo hướng đã phá</t>
+  </si>
+  <si>
+    <t>Xem ở phần nâng cao bên dưới</t>
+  </si>
+  <si>
+    <t>Nâng cao</t>
+  </si>
+  <si>
+    <t>Cơ bản</t>
+  </si>
+  <si>
+    <t>Giờ khi giá đã chạm vào đường MA55 thì ta sẽ thấy được các ngưỡng hỗ trợ và kháng cự xuất hiện bao khu vực này</t>
+  </si>
+  <si>
+    <t>Chú ý là phải chờ cho giá cắt qua đường MA55 thì mới hình thành các keylevel chuẩn nha, chưa cắt là thị trường vẫn tiếp tục chạy và chưa hình thành đâu</t>
+  </si>
+  <si>
+    <t>Đó là những đáy, đỉnh của những xu hướng lớn đã hình thành trước đó(keylevel)</t>
+  </si>
+  <si>
+    <t>Bắt những pha khi thị trường phá keylevel</t>
+  </si>
+  <si>
+    <t>Vào lệnh khi giá phá keylevel (Cơ bản)</t>
+  </si>
+  <si>
+    <t>Do giao dịch trong khung thời gian ngắn nhưng keylevel ít nhất phải được hình thành bởi khung H1, nếu sử dụng keylevel bởi khung M15 thì nó có sức mạnh khá yếu</t>
+  </si>
+  <si>
+    <t>Ngoài ra chúng ta phải chú ý đến những keylevel được hình thành bởi những khung thời gian lớn hơn nếu như giá đi đến gần khung đó</t>
+  </si>
+  <si>
+    <t>có thế ta sẽ vẽ những keylevel của những khung thời gian khác nhau theo độ lớn của khung vẽ</t>
+  </si>
+  <si>
+    <t>khung thời gian M15 hay chỉ dùng để tìm điểm vào lệnh khi giá đi đến vùng keylevel thôi</t>
+  </si>
+  <si>
+    <t>Ta phải chờ khi giá vào vùng keylevel và chờ xuất hiện loại nến đảo chiều này</t>
+  </si>
+  <si>
+    <t>Keylevel được hình thành bởi khung càng lớn thì sức mạnh càng cao</t>
+  </si>
+  <si>
+    <t>Khi tác động vào keylevel mà bật lại thì nó sẽ đi đến vùng sinh ra nó</t>
+  </si>
+  <si>
+    <t>Do đó vùng sinh ra bởi khung D1 sẽ lớn hơn H4, H4 lớn hơn H1…</t>
+  </si>
+  <si>
+    <t>Để tăng cường vị thế khi vào lệnh thì tại vùng keylevel phải có nến H1 đảo chiều(do dao dịch trong khung nhỏ(M15) thì cần ít nhất là nến H1 đảo chiều làm điểm tựa cho keylevel đó)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +531,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -426,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -435,6 +569,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,13 +648,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>152</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>517208</xdr:colOff>
-      <xdr:row>191</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>175140</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -551,13 +686,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>16008</xdr:colOff>
-      <xdr:row>218</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>36018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>106632</xdr:colOff>
-      <xdr:row>263</xdr:row>
+      <xdr:row>269</xdr:row>
       <xdr:rowOff>34946</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -587,15 +722,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>421824</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>599393</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -615,6 +750,44 @@
         <a:xfrm>
           <a:off x="8886650" y="23680946"/>
           <a:ext cx="5080873" cy="2856531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>199801</xdr:colOff>
+      <xdr:row>319</xdr:row>
+      <xdr:rowOff>32546</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="627530" y="52286647"/>
+          <a:ext cx="15238095" cy="8571428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -889,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:O356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q214" sqref="Q214"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K333" sqref="K333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="90" x14ac:dyDescent="1.1499999999999999">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1044,7 +1217,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1057,7 +1230,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1069,7 +1242,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1081,7 +1254,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1092,7 +1265,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1103,7 +1276,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1114,7 +1287,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1125,7 +1298,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1136,7 +1309,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1147,7 +1320,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1158,7 +1331,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1169,7 +1342,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1196,7 +1369,7 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -1206,425 +1379,631 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>10</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B91" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C94" t="s">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D101" t="s">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>60</v>
+      </c>
+      <c r="G106" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="113" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>20</v>
+      </c>
+      <c r="G116" t="s">
+        <v>23</v>
+      </c>
+      <c r="M116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>21</v>
+      </c>
+      <c r="G117" t="s">
+        <v>22</v>
+      </c>
+      <c r="M117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="119" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="121" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="123" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="125" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="131" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="136" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="137" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>40</v>
+      </c>
+      <c r="J137" t="s">
+        <v>41</v>
+      </c>
+      <c r="N137" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="138" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>35</v>
+      </c>
+      <c r="J138" t="s">
+        <v>42</v>
+      </c>
+      <c r="N138" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="139" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>36</v>
+      </c>
+      <c r="N139" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="140" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>37</v>
+      </c>
+      <c r="N140" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="141" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>38</v>
+      </c>
+      <c r="N141" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="N142" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="143" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="144" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="201" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="202" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C202" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="104" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="105" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D105" t="s">
-        <v>63</v>
-      </c>
-      <c r="H105" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="107" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D107" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D109" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D111" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="112" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="113" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>22</v>
-      </c>
-      <c r="H113" t="s">
-        <v>25</v>
-      </c>
-      <c r="N113" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="114" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D114" t="s">
-        <v>23</v>
-      </c>
-      <c r="H114" t="s">
-        <v>24</v>
-      </c>
-      <c r="N114" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D115" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="116" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="118" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D118" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="120" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D120" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="121" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D121" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="122" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D122" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="126" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D126" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="127" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D127" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="128" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D128" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="130" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="131" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D131" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="132" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D132" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="133" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="E133" t="s">
+    <row r="203" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C203" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="134" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D134" t="s">
-        <v>42</v>
-      </c>
-      <c r="K134" t="s">
-        <v>43</v>
-      </c>
-      <c r="O134" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="135" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D135" t="s">
-        <v>37</v>
-      </c>
-      <c r="K135" t="s">
-        <v>44</v>
-      </c>
-      <c r="O135" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="136" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D136" t="s">
-        <v>38</v>
-      </c>
-      <c r="O136" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="137" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D137" t="s">
-        <v>39</v>
-      </c>
-      <c r="O137" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="138" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D138" t="s">
-        <v>40</v>
-      </c>
-      <c r="O138" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="139" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="O139" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="141" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D141" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="142" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D142" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="143" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D143" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="144" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D144" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="195" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B195" t="s">
+    <row r="204" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C204" t="s">
+        <v>73</v>
+      </c>
+      <c r="K204" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="205" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K205" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="207" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C207" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="210" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C210" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="196" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C196" t="s">
+    <row r="211" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C211" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="197" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C197" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="198" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C198" t="s">
-        <v>76</v>
-      </c>
-      <c r="K198" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="199" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K199" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="201" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C201" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="204" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C204" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C205" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C206" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="207" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C207" t="s">
-        <v>74</v>
-      </c>
-      <c r="J207" t="s">
-        <v>78</v>
-      </c>
-      <c r="O207" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="208" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C208" t="s">
-        <v>75</v>
-      </c>
-      <c r="O208" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="209" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="J209" t="s">
-        <v>79</v>
-      </c>
-      <c r="O209" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="210" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="O210" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="212" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="213" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C213" t="s">
-        <v>105</v>
+        <v>71</v>
+      </c>
+      <c r="J213" t="s">
+        <v>75</v>
+      </c>
+      <c r="O213" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="214" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
-        <v>107</v>
+        <v>72</v>
+      </c>
+      <c r="O214" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="215" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C215" t="s">
-        <v>110</v>
+      <c r="J215" t="s">
+        <v>76</v>
+      </c>
+      <c r="O215" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="216" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C216" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="217" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C217" t="s">
-        <v>109</v>
+      <c r="O216" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="218" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C218" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="219" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C219" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="220" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C220" t="s">
+        <v>103</v>
+      </c>
+      <c r="O220" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="221" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C221" t="s">
+        <v>106</v>
+      </c>
+      <c r="O221" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="222" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C222" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="223" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C223" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="322" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B322" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B324" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B333" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B346" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B349" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B352" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="354" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="355" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>130</v>
+      </c>
+      <c r="E355" t="s">
+        <v>131</v>
+      </c>
+      <c r="O355" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="356" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E356" t="s">
+        <v>132</v>
+      </c>
+      <c r="O356" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cap nhat ngay 10/10
</commit_message>
<xml_diff>
--- a/Breakout.xlsx
+++ b/Breakout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
   <si>
     <t>Người thực hiện:</t>
   </si>
@@ -490,6 +490,9 @@
   </si>
   <si>
     <t>Để tăng cường vị thế khi vào lệnh thì tại vùng keylevel phải có nến H1 đảo chiều(do dao dịch trong khung nhỏ(M15) thì cần ít nhất là nến H1 đảo chiều làm điểm tựa cho keylevel đó)</t>
+  </si>
+  <si>
+    <t>Tất cả các tài liệu chỉ viết ví dụ cho trường hợp là tăng, còn giảm thì cũng tương tự</t>
   </si>
 </sst>
 </file>
@@ -593,13 +596,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>173181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>4329</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -648,13 +651,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>154</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>517208</xdr:colOff>
-      <xdr:row>197</xdr:row>
+      <xdr:row>199</xdr:row>
       <xdr:rowOff>175140</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -686,13 +689,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>16008</xdr:colOff>
-      <xdr:row>224</xdr:row>
+      <xdr:row>226</xdr:row>
       <xdr:rowOff>36018</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>106632</xdr:colOff>
-      <xdr:row>269</xdr:row>
+      <xdr:row>271</xdr:row>
       <xdr:rowOff>34946</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -724,13 +727,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>421824</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>599393</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -762,13 +765,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>22412</xdr:colOff>
-      <xdr:row>274</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>199801</xdr:colOff>
-      <xdr:row>319</xdr:row>
+      <xdr:row>321</xdr:row>
       <xdr:rowOff>32546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1062,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O356"/>
+  <dimension ref="A1:O358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K333" sqref="K333"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,627 +1380,651 @@
       <c r="H25" s="4"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
+    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>59</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>146</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>107</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D40" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B91" s="6" t="s">
+    <row r="93" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B93" s="6" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C102" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>60</v>
-      </c>
-      <c r="G106" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="G108" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="113" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="115" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C115" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="116" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C116" t="s">
-        <v>20</v>
-      </c>
-      <c r="G116" t="s">
-        <v>23</v>
-      </c>
-      <c r="M116" t="s">
-        <v>24</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C117" t="s">
-        <v>21</v>
-      </c>
-      <c r="G117" t="s">
-        <v>22</v>
-      </c>
-      <c r="M117" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="118" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C118" t="s">
-        <v>58</v>
+        <v>20</v>
+      </c>
+      <c r="G118" t="s">
+        <v>23</v>
+      </c>
+      <c r="M118" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C119" t="s">
-        <v>79</v>
+        <v>21</v>
+      </c>
+      <c r="G119" t="s">
+        <v>22</v>
+      </c>
+      <c r="M119" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="121" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
     </row>
     <row r="123" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="124" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C124" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="127" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C129" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="130" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C130" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="131" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="132" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="133" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C133" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C134" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="135" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="D136" t="s">
-        <v>65</v>
+      <c r="C136" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="137" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>40</v>
-      </c>
-      <c r="J137" t="s">
-        <v>41</v>
-      </c>
-      <c r="N137" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C138" t="s">
-        <v>35</v>
-      </c>
-      <c r="J138" t="s">
-        <v>42</v>
-      </c>
-      <c r="N138" t="s">
-        <v>43</v>
+      <c r="D138" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="139" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="J139" t="s">
+        <v>41</v>
       </c>
       <c r="N139" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="140" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="J140" t="s">
+        <v>42</v>
       </c>
       <c r="N140" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="141" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C141" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N141" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>37</v>
+      </c>
       <c r="N142" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="143" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C143" t="s">
-        <v>138</v>
+        <v>38</v>
+      </c>
+      <c r="N143" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="144" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C144" t="s">
-        <v>139</v>
+      <c r="N144" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C145" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C147" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C148" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C149" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C150" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="201" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
+    <row r="203" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="202" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C202" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="203" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C203" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="204" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="205" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C205" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="206" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C206" t="s">
         <v>73</v>
       </c>
-      <c r="K204" t="s">
+      <c r="K206" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="205" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K205" t="s">
+    <row r="207" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K207" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="207" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C207" t="s">
+    <row r="209" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C209" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="210" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C210" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="211" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C211" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="212" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C212" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="213" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C213" t="s">
-        <v>71</v>
-      </c>
-      <c r="J213" t="s">
-        <v>75</v>
-      </c>
-      <c r="O213" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="214" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="215" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C215" t="s">
+        <v>71</v>
+      </c>
+      <c r="J215" t="s">
+        <v>75</v>
+      </c>
+      <c r="O215" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="216" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C216" t="s">
         <v>72</v>
       </c>
-      <c r="O214" t="s">
+      <c r="O216" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="215" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="J215" t="s">
+    <row r="217" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="J217" t="s">
         <v>76</v>
       </c>
-      <c r="O215" t="s">
+      <c r="O217" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="216" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="O216" t="s">
+    <row r="218" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O218" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="218" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C218" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="219" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C219" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="220" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
-        <v>103</v>
-      </c>
-      <c r="O220" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
     </row>
     <row r="221" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
-        <v>106</v>
-      </c>
-      <c r="O221" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
     </row>
     <row r="222" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="O222" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="223" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
+        <v>106</v>
+      </c>
+      <c r="O223" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="224" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C224" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C225" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B272" t="s">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B273" t="s">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="322" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B322" s="6" t="s">
+    <row r="324" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B324" s="6" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="324" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B324" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="325" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B325" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="327" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="328" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="329" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="330" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="331" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="332" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="333" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="334" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="335" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="336" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="337" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="338" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
     </row>
     <row r="339" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="340" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="341" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B342" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="343" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B344" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="345" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="346" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="347" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B348" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="349" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B350" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="351" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="352" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="353" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="354" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="356" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="355" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B355" t="s">
+    <row r="357" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
         <v>130</v>
       </c>
-      <c r="E355" t="s">
+      <c r="E357" t="s">
         <v>131</v>
       </c>
-      <c r="O355" t="s">
+      <c r="O357" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="356" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E356" t="s">
+    <row r="358" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E358" t="s">
         <v>132</v>
       </c>
-      <c r="O356" t="s">
+      <c r="O358" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cap nhat canh buy
</commit_message>
<xml_diff>
--- a/Breakout.xlsx
+++ b/Breakout.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="159">
   <si>
     <t>Người thực hiện:</t>
   </si>
@@ -493,13 +493,16 @@
   </si>
   <si>
     <t>Tất cả các tài liệu chỉ viết ví dụ cho trường hợp là tăng, còn giảm thì cũng tương tự</t>
+  </si>
+  <si>
+    <t>Lĩnh ngộ tinh túy thị trường</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +545,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -563,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -573,6 +584,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1289,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>91</v>
       </c>
@@ -1288,7 +1300,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>92</v>
       </c>
@@ -1299,7 +1311,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>93</v>
       </c>
@@ -1310,7 +1322,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>97</v>
       </c>
@@ -1321,7 +1333,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>94</v>
       </c>
@@ -1332,7 +1344,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>96</v>
       </c>
@@ -1343,7 +1355,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>95</v>
       </c>
@@ -1354,7 +1366,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1365,7 +1377,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>9</v>
       </c>
@@ -1379,8 +1391,11 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J25" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1391,7 +1406,7 @@
       <c r="H26" s="4"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>157</v>
@@ -1404,22 +1419,22 @@
       <c r="H27" s="4"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>52</v>
       </c>

</xml_diff>